<commit_message>
Fixed v2.0 bug 2: id map not saving properly
</commit_message>
<xml_diff>
--- a/Spend.xlsx
+++ b/Spend.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaysondale/Statement-Analyzer-GUI-V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA2413D-9249-9142-B212-97483389EDA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DF0170-87DA-A344-995B-5F2EB6FB55E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31720" yWindow="-2220" windowWidth="27640" windowHeight="16540" xr2:uid="{09CAAE6D-E5E1-6C4B-BC1B-E464361E21CC}"/>
   </bookViews>
   <sheets>
-    <sheet name="V2.0" sheetId="1" r:id="rId1"/>
+    <sheet name="Features" sheetId="2" r:id="rId1"/>
+    <sheet name="Bugs V2.0" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Spend Bug Report</t>
   </si>
@@ -83,6 +84,57 @@
   </si>
   <si>
     <t>HIGH</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Commit</t>
+  </si>
+  <si>
+    <t>f2aeae5ef920ec3fdea608e5de2329cda4c40e27</t>
+  </si>
+  <si>
+    <t>Commit ID</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Issue occurred when the transaction id string contained a comma value which mess up the transaction line indexiing.
+Fixed by centralizing the transaction format (created BankFormat enum) and checking to make sure each line item was the appropriate length before proceeding to parse values. If the actual length does not match the desired length, the line is shorteded by merging the id string and the adjacent string.
+Future Risk: The system may encounter an issue if any further formatting issues occur (ie. numbers in the wrong place)</t>
+  </si>
+  <si>
+    <t>Statement Loading Pt. 2</t>
+  </si>
+  <si>
+    <t>Changing the name of the file seemed to allow statements to be imported.
+Error could also be due to table not refreshing (cannot confirm that values were not imported and simply not being displayed)</t>
+  </si>
+  <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>Spend Features</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>BMO Compatibility</t>
+  </si>
+  <si>
+    <t>Make BMO Statements Compatible with System by adding to BankFormat Enum structure</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Release Version</t>
   </si>
 </sst>
 </file>
@@ -183,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -206,38 +258,208 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -546,11 +768,545 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8ACDC5-E237-9846-92A5-7DAC37E4427B}">
-  <dimension ref="C2:H44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46691BE8-5819-B147-BF07-ECD0D968A0B2}">
+  <dimension ref="C2:H61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.33203125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="59.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C2" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C5" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="88" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="26">
+        <v>2.1</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="27"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C7" s="26"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C8" s="26"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C9" s="26"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C10" s="26"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="26"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="26"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="26"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="26"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="26"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C16" s="26"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="26"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="26"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="26"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="26"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="26"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="26"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C23" s="26"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C24" s="26"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C25" s="26"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C26" s="26"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C27" s="26"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C28" s="26"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C29" s="26"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C30" s="26"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C31" s="26"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C32" s="26"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C33" s="26"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C34" s="26"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="8"/>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C35" s="26"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C36" s="26"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C37" s="26"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C38" s="26"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C39" s="26"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="8"/>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C40" s="26"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="8"/>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C41" s="26"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="8"/>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C42" s="26"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C43" s="26"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="8"/>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C44" s="26"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="8"/>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C45" s="26"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="8"/>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C46" s="26"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C47" s="26"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C48" s="26"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C49" s="26"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="8"/>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C50" s="26"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="8"/>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C51" s="26"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="8"/>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C52" s="26"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="8"/>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C53" s="26"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="8"/>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C54" s="26"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="8"/>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C55" s="26"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="8"/>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C56" s="26"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="8"/>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C57" s="26"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="8"/>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C58" s="26"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="8"/>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C59" s="26"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="8"/>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C60" s="26"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="8"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="8"/>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C61" s="26"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:H2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Not Started">
+      <formula>NOT(ISERROR(SEARCH("Not Started",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8ACDC5-E237-9846-92A5-7DAC37E4427B}">
+  <dimension ref="C2:J44"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,21 +1314,25 @@
     <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14" style="18" customWidth="1"/>
+    <col min="7" max="7" width="14" style="16" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="67.5" customWidth="1"/>
+    <col min="10" max="10" width="40.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C2" s="13" t="s">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
@@ -581,10 +1341,12 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="15"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="6"/>
+      <c r="J3" s="19"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
@@ -593,10 +1355,12 @@
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="15"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="6"/>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="6"/>
+      <c r="J4" s="19"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
@@ -609,338 +1373,429 @@
       <c r="F6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="3:8" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="8">
         <v>1</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="8">
         <v>2</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="20"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="3:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="C9" s="8">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="20"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="12"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="14"/>
+      <c r="G10" s="12"/>
       <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="20"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="12"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="12"/>
       <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="20"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="12"/>
+      <c r="E12" s="11"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="14"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="20"/>
+      <c r="J12" s="18"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="12"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="14"/>
+      <c r="G13" s="12"/>
       <c r="H13" s="10"/>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="20"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="12"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="14"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="10"/>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="20"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="12"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="14"/>
+      <c r="G15" s="12"/>
       <c r="H15" s="10"/>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="20"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="12"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="14"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="20"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="12"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="14"/>
+      <c r="G17" s="12"/>
       <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="20"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="12"/>
+      <c r="E18" s="11"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="14"/>
+      <c r="G18" s="12"/>
       <c r="H18" s="10"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="20"/>
+      <c r="J18" s="18"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="12"/>
+      <c r="E19" s="11"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="14"/>
+      <c r="G19" s="12"/>
       <c r="H19" s="10"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="20"/>
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="12"/>
+      <c r="E20" s="11"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="14"/>
+      <c r="G20" s="12"/>
       <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="20"/>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="12"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="14"/>
+      <c r="G21" s="12"/>
       <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="20"/>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="12"/>
+      <c r="E22" s="11"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="14"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="10"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="20"/>
+      <c r="J22" s="18"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="12"/>
+      <c r="E23" s="11"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="14"/>
+      <c r="G23" s="12"/>
       <c r="H23" s="10"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="20"/>
+      <c r="J23" s="18"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="12"/>
+      <c r="E24" s="11"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="14"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="20"/>
+      <c r="J24" s="18"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="12"/>
+      <c r="E25" s="11"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="14"/>
+      <c r="G25" s="12"/>
       <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="20"/>
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="12"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="14"/>
+      <c r="G26" s="12"/>
       <c r="H26" s="10"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="20"/>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="12"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="14"/>
+      <c r="G27" s="12"/>
       <c r="H27" s="10"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="20"/>
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="12"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="14"/>
+      <c r="G28" s="12"/>
       <c r="H28" s="10"/>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="20"/>
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="12"/>
+      <c r="E29" s="11"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="14"/>
+      <c r="G29" s="12"/>
       <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="20"/>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="12"/>
+      <c r="E30" s="11"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="14"/>
+      <c r="G30" s="12"/>
       <c r="H30" s="10"/>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="20"/>
+      <c r="J30" s="18"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="12"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="14"/>
+      <c r="G31" s="12"/>
       <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="20"/>
+      <c r="J31" s="18"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="12"/>
+      <c r="E32" s="11"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="14"/>
+      <c r="G32" s="12"/>
       <c r="H32" s="10"/>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="20"/>
+      <c r="J32" s="18"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="12"/>
+      <c r="E33" s="11"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="14"/>
+      <c r="G33" s="12"/>
       <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="20"/>
+      <c r="J33" s="18"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
-      <c r="E34" s="12"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="9"/>
-      <c r="G34" s="14"/>
+      <c r="G34" s="12"/>
       <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="20"/>
+      <c r="J34" s="18"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="12"/>
+      <c r="E35" s="11"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="14"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="10"/>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="20"/>
+      <c r="J35" s="18"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="12"/>
+      <c r="E36" s="11"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="14"/>
+      <c r="G36" s="12"/>
       <c r="H36" s="10"/>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="20"/>
+      <c r="J36" s="18"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="2"/>
       <c r="F37" s="3"/>
-      <c r="G37" s="17"/>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G37" s="15"/>
+      <c r="H37" s="21"/>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="2"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="17"/>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G38" s="15"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="2"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="17"/>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G39" s="15"/>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="2"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="17"/>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G40" s="15"/>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="2"/>
       <c r="F41" s="3"/>
-      <c r="G41" s="17"/>
-    </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G41" s="15"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="2"/>
       <c r="F42" s="3"/>
-      <c r="G42" s="17"/>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G42" s="15"/>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="2"/>
       <c r="F43" s="3"/>
-      <c r="G43" s="17"/>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="G43" s="15"/>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="2"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="17"/>
+      <c r="G44" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C2:J2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Unresolved">
+      <formula>NOT(ISERROR(SEARCH("Unresolved",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Fixed">
+      <formula>NOT(ISERROR(SEARCH("Fixed",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refresh transaction table after importing statements
</commit_message>
<xml_diff>
--- a/Spend.xlsx
+++ b/Spend.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaysondale/Statement-Analyzer-GUI-V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DF0170-87DA-A344-995B-5F2EB6FB55E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FAD15D-7AD8-A34D-BDD2-A7350341A426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31720" yWindow="-2220" windowWidth="27640" windowHeight="16540" xr2:uid="{09CAAE6D-E5E1-6C4B-BC1B-E464361E21CC}"/>
+    <workbookView xWindow="2900" yWindow="1380" windowWidth="27640" windowHeight="16540" xr2:uid="{09CAAE6D-E5E1-6C4B-BC1B-E464361E21CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="2" r:id="rId1"/>
     <sheet name="Bugs V2.0" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Spend Bug Report</t>
   </si>
@@ -135,6 +135,39 @@
   </si>
   <si>
     <t>Release Version</t>
+  </si>
+  <si>
+    <t>19989a3d5e115553033ba4d182897c5963414e9e</t>
+  </si>
+  <si>
+    <t>Fixed mapping function call to ensure id maps are added properly to the hashmap</t>
+  </si>
+  <si>
+    <t>Transaction Hashing</t>
+  </si>
+  <si>
+    <t>Make all transaction have unique hashing outcome by passing more information into the hash function. Avoid all conflicts</t>
+  </si>
+  <si>
+    <t>04-15-2020</t>
+  </si>
+  <si>
+    <t>Saving Statement Directory</t>
+  </si>
+  <si>
+    <t>User should not need to import statements every time</t>
+  </si>
+  <si>
+    <t>Auto-Detect Statement Type</t>
+  </si>
+  <si>
+    <t>User should be able to have different types of bank statements in the import directory and have all loaded properly</t>
+  </si>
+  <si>
+    <t>Set Category Appearance Order</t>
+  </si>
+  <si>
+    <t>Allow user to reorganize the order of category labels for optimal convenience</t>
   </si>
 </sst>
 </file>
@@ -214,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -231,11 +264,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -304,11 +346,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -386,76 +437,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -772,13 +753,13 @@
   <dimension ref="C2:H61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="14.33203125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
     <col min="5" max="5" width="47.83203125" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="59.5" customWidth="1"/>
@@ -799,7 +780,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -827,7 +808,7 @@
       </c>
     </row>
     <row r="6" spans="3:8" ht="88" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="26">
+      <c r="C6" s="29">
         <v>2.1</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -842,35 +823,61 @@
       <c r="G6" s="27"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C7" s="26"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="8"/>
+    <row r="7" spans="3:8" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="28"/>
+      <c r="D7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="G7" s="27"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C8" s="26"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="8"/>
+    <row r="8" spans="3:8" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="30">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="G8" s="27"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C9" s="26"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8"/>
+    <row r="9" spans="3:8" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="29"/>
+      <c r="D9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="G9" s="27"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C10" s="26"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="8"/>
+    <row r="10" spans="3:8" ht="92" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="28"/>
+      <c r="D10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="G10" s="27"/>
       <c r="H10" s="8"/>
     </row>
@@ -1283,8 +1290,10 @@
       <c r="H61" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Not Started">
@@ -1306,7 +1315,7 @@
   <dimension ref="C2:J44"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1351,7 +1360,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -1429,10 +1438,14 @@
         <v>15</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="20"/>
-      <c r="J8" s="18"/>
+        <v>16</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="3:10" ht="68" x14ac:dyDescent="0.2">
       <c r="C9" s="8">

</xml_diff>